<commit_message>
Add CV and ROC analysis
</commit_message>
<xml_diff>
--- a/health/scores/folds_10sf.xlsx
+++ b/health/scores/folds_10sf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="10sf_fold_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="28">
   <si>
     <t xml:space="preserve">FID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">Obesidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predicted</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -112,11 +115,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,6 +150,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,11 +221,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -291,7 +309,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -325,6 +343,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -434,6 +453,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -521,11 +541,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="46315586"/>
-        <c:axId val="42390507"/>
+        <c:axId val="40431708"/>
+        <c:axId val="90915226"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46315586"/>
+        <c:axId val="40431708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,14 +580,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42390507"/>
+        <c:crossAx val="90915226"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42390507"/>
+        <c:axId val="90915226"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +602,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -611,7 +631,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46315586"/>
+        <c:crossAx val="40431708"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -659,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -669,8 +689,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5110920" y="2706120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="5034960" y="2706120"/>
+        <a:ext cx="5670000" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -688,15 +708,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T114"/>
+  <dimension ref="A1:V114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V:V"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,6 +759,9 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -781,12 +804,17 @@
       <c r="M2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="N2" s="0" t="n">
+        <f aca="false">IF(L2&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
         <v>113</v>
       </c>
+      <c r="V2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -829,13 +857,18 @@
       <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="2" t="n">
+      <c r="N3" s="0" t="n">
+        <f aca="false">IF(L3&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <f aca="false">SUM(M2:M114)</f>
         <v>22</v>
       </c>
+      <c r="V3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -878,13 +911,18 @@
       <c r="M4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2" t="n">
+      <c r="N4" s="0" t="n">
+        <f aca="false">IF(L4&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <f aca="false">P3/P2</f>
         <v>0.194690265486726</v>
       </c>
+      <c r="V4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -927,12 +965,17 @@
       <c r="M5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="n">
+      <c r="N5" s="0" t="n">
+        <f aca="false">IF(L5&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="V5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -975,27 +1018,32 @@
       <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2" t="n">
+      <c r="N6" s="0" t="n">
+        <f aca="false">IF(L6&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <f aca="false">P5*P4</f>
         <v>2.33628318584071</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2" t="n">
+      <c r="Q6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <f aca="false">(P3/P2)*(1 - (P3/P2))*P5*((P2-P5)/(P2-1))</f>
         <v>1.69664813219516</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="2" t="n">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="3" t="n">
         <f aca="false">SQRT(R6)</f>
         <v>1.30255446419532</v>
       </c>
+      <c r="V6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1038,22 +1086,27 @@
       <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="N7" s="0" t="n">
+        <f aca="false">IF(L7&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <f aca="false">COUNTIF(M2:M13, "=1")</f>
         <v>2</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="n">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3" t="n">
         <f aca="false">P6+2*T6</f>
         <v>4.94139211423135</v>
       </c>
+      <c r="V7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1096,10 +1149,15 @@
       <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="N8" s="0" t="n">
+        <f aca="false">IF(L8&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="V8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1142,17 +1200,22 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="N9" s="0" t="n">
+        <f aca="false">IF(L9&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="n">
         <f aca="false">P7/P6 - 1</f>
         <v>-0.143939393939394</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="V9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1195,6 +1258,11 @@
       <c r="M10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">IF(L10&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1237,15 +1305,20 @@
       <c r="M11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false">IF(L11&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="V11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1288,6 +1361,10 @@
       <c r="M12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N12" s="0" t="n">
+        <f aca="false">IF(L12&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O12" s="0" t="n">
         <v>10</v>
       </c>
@@ -1299,6 +1376,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1341,6 +1419,10 @@
       <c r="M13" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">IF(L13&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O13" s="0" t="n">
         <v>20</v>
       </c>
@@ -1352,6 +1434,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1394,6 +1477,10 @@
       <c r="M14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">IF(L14&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O14" s="0" t="n">
         <v>30</v>
       </c>
@@ -1405,6 +1492,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1447,6 +1535,10 @@
       <c r="M15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">IF(L15&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O15" s="0" t="n">
         <v>40</v>
       </c>
@@ -1458,6 +1550,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1500,6 +1593,10 @@
       <c r="M16" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">IF(L16&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O16" s="0" t="n">
         <v>50</v>
       </c>
@@ -1511,6 +1608,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1553,6 +1651,10 @@
       <c r="M17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">IF(L17&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O17" s="0" t="n">
         <v>60</v>
       </c>
@@ -1564,6 +1666,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1606,6 +1709,10 @@
       <c r="M18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">IF(L18&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O18" s="0" t="n">
         <v>70</v>
       </c>
@@ -1617,6 +1724,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -1659,6 +1767,10 @@
       <c r="M19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N19" s="0" t="n">
+        <f aca="false">IF(L19&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O19" s="0" t="n">
         <v>80</v>
       </c>
@@ -1670,6 +1782,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1712,6 +1825,10 @@
       <c r="M20" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">IF(L20&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O20" s="0" t="n">
         <v>90</v>
       </c>
@@ -1723,6 +1840,7 @@
         <f aca="false">$P$3*11/$P$2</f>
         <v>2.14159292035398</v>
       </c>
+      <c r="V20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1765,6 +1883,10 @@
       <c r="M21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">IF(L21&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="O21" s="0" t="n">
         <v>100</v>
       </c>
@@ -1776,6 +1898,7 @@
         <f aca="false">$P$3*14/$P$2</f>
         <v>2.72566371681416</v>
       </c>
+      <c r="V21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1818,6 +1941,11 @@
       <c r="M22" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N22" s="0" t="n">
+        <f aca="false">IF(L22&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1860,6 +1988,11 @@
       <c r="M23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">IF(L23&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -1902,6 +2035,11 @@
       <c r="M24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N24" s="0" t="n">
+        <f aca="false">IF(L24&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -1944,6 +2082,11 @@
       <c r="M25" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">IF(L25&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1986,6 +2129,11 @@
       <c r="M26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N26" s="0" t="n">
+        <f aca="false">IF(L26&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -2028,6 +2176,11 @@
       <c r="M27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">IF(L27&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -2070,6 +2223,11 @@
       <c r="M28" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N28" s="0" t="n">
+        <f aca="false">IF(L28&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -2112,6 +2270,11 @@
       <c r="M29" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">IF(L29&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -2154,6 +2317,11 @@
       <c r="M30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">IF(L30&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -2196,6 +2364,11 @@
       <c r="M31" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N31" s="0" t="n">
+        <f aca="false">IF(L31&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -2238,6 +2411,11 @@
       <c r="M32" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N32" s="0" t="n">
+        <f aca="false">IF(L32&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -2280,6 +2458,11 @@
       <c r="M33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N33" s="0" t="n">
+        <f aca="false">IF(L33&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -2322,6 +2505,11 @@
       <c r="M34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N34" s="0" t="n">
+        <f aca="false">IF(L34&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -2364,6 +2552,11 @@
       <c r="M35" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N35" s="0" t="n">
+        <f aca="false">IF(L35&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -2406,6 +2599,11 @@
       <c r="M36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N36" s="0" t="n">
+        <f aca="false">IF(L36&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -2448,6 +2646,11 @@
       <c r="M37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N37" s="0" t="n">
+        <f aca="false">IF(L37&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -2490,6 +2693,11 @@
       <c r="M38" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N38" s="0" t="n">
+        <f aca="false">IF(L38&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -2532,6 +2740,11 @@
       <c r="M39" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N39" s="0" t="n">
+        <f aca="false">IF(L39&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -2574,6 +2787,11 @@
       <c r="M40" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N40" s="0" t="n">
+        <f aca="false">IF(L40&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -2616,6 +2834,11 @@
       <c r="M41" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N41" s="0" t="n">
+        <f aca="false">IF(L41&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -2658,6 +2881,11 @@
       <c r="M42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N42" s="0" t="n">
+        <f aca="false">IF(L42&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -2700,6 +2928,11 @@
       <c r="M43" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N43" s="0" t="n">
+        <f aca="false">IF(L43&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2742,6 +2975,11 @@
       <c r="M44" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N44" s="0" t="n">
+        <f aca="false">IF(L44&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -2784,6 +3022,11 @@
       <c r="M45" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N45" s="0" t="n">
+        <f aca="false">IF(L45&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -2826,6 +3069,11 @@
       <c r="M46" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N46" s="0" t="n">
+        <f aca="false">IF(L46&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -2868,6 +3116,11 @@
       <c r="M47" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N47" s="0" t="n">
+        <f aca="false">IF(L47&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -2910,6 +3163,11 @@
       <c r="M48" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N48" s="0" t="n">
+        <f aca="false">IF(L48&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -2952,6 +3210,11 @@
       <c r="M49" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N49" s="0" t="n">
+        <f aca="false">IF(L49&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -2994,6 +3257,11 @@
       <c r="M50" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N50" s="0" t="n">
+        <f aca="false">IF(L50&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -3036,6 +3304,11 @@
       <c r="M51" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N51" s="0" t="n">
+        <f aca="false">IF(L51&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -3078,6 +3351,11 @@
       <c r="M52" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N52" s="0" t="n">
+        <f aca="false">IF(L52&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -3120,6 +3398,11 @@
       <c r="M53" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N53" s="0" t="n">
+        <f aca="false">IF(L53&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -3162,6 +3445,11 @@
       <c r="M54" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N54" s="0" t="n">
+        <f aca="false">IF(L54&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -3204,6 +3492,11 @@
       <c r="M55" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N55" s="0" t="n">
+        <f aca="false">IF(L55&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -3246,6 +3539,11 @@
       <c r="M56" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N56" s="0" t="n">
+        <f aca="false">IF(L56&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -3288,6 +3586,11 @@
       <c r="M57" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N57" s="0" t="n">
+        <f aca="false">IF(L57&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -3330,6 +3633,11 @@
       <c r="M58" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N58" s="0" t="n">
+        <f aca="false">IF(L58&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -3372,6 +3680,11 @@
       <c r="M59" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N59" s="0" t="n">
+        <f aca="false">IF(L59&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -3414,6 +3727,11 @@
       <c r="M60" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N60" s="0" t="n">
+        <f aca="false">IF(L60&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -3456,6 +3774,11 @@
       <c r="M61" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N61" s="0" t="n">
+        <f aca="false">IF(L61&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -3498,6 +3821,11 @@
       <c r="M62" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N62" s="0" t="n">
+        <f aca="false">IF(L62&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -3540,6 +3868,11 @@
       <c r="M63" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N63" s="0" t="n">
+        <f aca="false">IF(L63&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -3582,6 +3915,11 @@
       <c r="M64" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N64" s="0" t="n">
+        <f aca="false">IF(L64&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -3624,6 +3962,11 @@
       <c r="M65" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N65" s="0" t="n">
+        <f aca="false">IF(L65&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V65" s="4"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -3666,6 +4009,11 @@
       <c r="M66" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N66" s="0" t="n">
+        <f aca="false">IF(L66&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="4"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -3708,6 +4056,11 @@
       <c r="M67" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N67" s="0" t="n">
+        <f aca="false">IF(L67&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -3750,6 +4103,11 @@
       <c r="M68" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N68" s="0" t="n">
+        <f aca="false">IF(L68&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -3792,6 +4150,11 @@
       <c r="M69" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N69" s="0" t="n">
+        <f aca="false">IF(L69&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V69" s="4"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -3834,6 +4197,11 @@
       <c r="M70" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N70" s="0" t="n">
+        <f aca="false">IF(L70&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -3876,6 +4244,11 @@
       <c r="M71" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N71" s="0" t="n">
+        <f aca="false">IF(L71&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -3918,6 +4291,11 @@
       <c r="M72" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N72" s="0" t="n">
+        <f aca="false">IF(L72&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -3960,6 +4338,11 @@
       <c r="M73" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N73" s="0" t="n">
+        <f aca="false">IF(L73&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V73" s="4"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
@@ -4002,6 +4385,11 @@
       <c r="M74" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N74" s="0" t="n">
+        <f aca="false">IF(L74&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -4044,6 +4432,11 @@
       <c r="M75" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N75" s="0" t="n">
+        <f aca="false">IF(L75&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -4086,6 +4479,11 @@
       <c r="M76" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N76" s="0" t="n">
+        <f aca="false">IF(L76&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -4128,6 +4526,11 @@
       <c r="M77" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N77" s="0" t="n">
+        <f aca="false">IF(L77&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
@@ -4170,6 +4573,11 @@
       <c r="M78" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N78" s="0" t="n">
+        <f aca="false">IF(L78&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
@@ -4212,6 +4620,11 @@
       <c r="M79" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N79" s="0" t="n">
+        <f aca="false">IF(L79&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
@@ -4254,6 +4667,11 @@
       <c r="M80" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N80" s="0" t="n">
+        <f aca="false">IF(L80&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -4296,6 +4714,11 @@
       <c r="M81" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N81" s="0" t="n">
+        <f aca="false">IF(L81&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V81" s="4"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -4338,6 +4761,11 @@
       <c r="M82" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N82" s="0" t="n">
+        <f aca="false">IF(L82&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
@@ -4380,6 +4808,11 @@
       <c r="M83" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N83" s="0" t="n">
+        <f aca="false">IF(L83&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -4422,6 +4855,11 @@
       <c r="M84" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N84" s="0" t="n">
+        <f aca="false">IF(L84&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -4464,6 +4902,11 @@
       <c r="M85" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N85" s="0" t="n">
+        <f aca="false">IF(L85&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
@@ -4506,6 +4949,11 @@
       <c r="M86" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N86" s="0" t="n">
+        <f aca="false">IF(L86&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
@@ -4548,6 +4996,11 @@
       <c r="M87" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N87" s="0" t="n">
+        <f aca="false">IF(L87&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
@@ -4590,6 +5043,11 @@
       <c r="M88" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N88" s="0" t="n">
+        <f aca="false">IF(L88&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
@@ -4632,6 +5090,11 @@
       <c r="M89" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N89" s="0" t="n">
+        <f aca="false">IF(L89&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
@@ -4674,6 +5137,11 @@
       <c r="M90" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N90" s="0" t="n">
+        <f aca="false">IF(L90&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V90" s="4"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
@@ -4716,6 +5184,11 @@
       <c r="M91" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N91" s="0" t="n">
+        <f aca="false">IF(L91&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V91" s="4"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
@@ -4758,6 +5231,11 @@
       <c r="M92" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N92" s="0" t="n">
+        <f aca="false">IF(L92&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V92" s="4"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
@@ -4800,6 +5278,11 @@
       <c r="M93" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N93" s="0" t="n">
+        <f aca="false">IF(L93&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V93" s="4"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
@@ -4842,6 +5325,11 @@
       <c r="M94" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N94" s="0" t="n">
+        <f aca="false">IF(L94&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V94" s="4"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
@@ -4884,6 +5372,11 @@
       <c r="M95" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N95" s="0" t="n">
+        <f aca="false">IF(L95&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V95" s="4"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
@@ -4926,6 +5419,11 @@
       <c r="M96" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N96" s="0" t="n">
+        <f aca="false">IF(L96&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
@@ -4968,6 +5466,11 @@
       <c r="M97" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N97" s="0" t="n">
+        <f aca="false">IF(L97&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V97" s="4"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
@@ -5010,6 +5513,11 @@
       <c r="M98" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N98" s="0" t="n">
+        <f aca="false">IF(L98&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
@@ -5052,6 +5560,11 @@
       <c r="M99" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N99" s="0" t="n">
+        <f aca="false">IF(L99&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
@@ -5094,6 +5607,11 @@
       <c r="M100" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N100" s="0" t="n">
+        <f aca="false">IF(L100&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
@@ -5136,6 +5654,11 @@
       <c r="M101" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N101" s="0" t="n">
+        <f aca="false">IF(L101&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
@@ -5178,6 +5701,11 @@
       <c r="M102" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N102" s="0" t="n">
+        <f aca="false">IF(L102&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V102" s="4"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
@@ -5220,6 +5748,11 @@
       <c r="M103" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N103" s="0" t="n">
+        <f aca="false">IF(L103&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V103" s="4"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
@@ -5262,6 +5795,11 @@
       <c r="M104" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N104" s="0" t="n">
+        <f aca="false">IF(L104&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V104" s="4"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
@@ -5304,6 +5842,11 @@
       <c r="M105" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N105" s="0" t="n">
+        <f aca="false">IF(L105&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V105" s="4"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
@@ -5346,6 +5889,11 @@
       <c r="M106" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N106" s="0" t="n">
+        <f aca="false">IF(L106&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V106" s="4"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
@@ -5388,6 +5936,11 @@
       <c r="M107" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N107" s="0" t="n">
+        <f aca="false">IF(L107&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V107" s="4"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
@@ -5430,6 +5983,11 @@
       <c r="M108" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N108" s="0" t="n">
+        <f aca="false">IF(L108&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
@@ -5472,6 +6030,11 @@
       <c r="M109" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N109" s="0" t="n">
+        <f aca="false">IF(L109&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V109" s="4"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
@@ -5514,6 +6077,11 @@
       <c r="M110" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N110" s="0" t="n">
+        <f aca="false">IF(L110&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V110" s="4"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
@@ -5556,6 +6124,11 @@
       <c r="M111" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N111" s="0" t="n">
+        <f aca="false">IF(L111&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
@@ -5598,6 +6171,11 @@
       <c r="M112" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N112" s="0" t="n">
+        <f aca="false">IF(L112&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
@@ -5640,6 +6218,11 @@
       <c r="M113" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N113" s="0" t="n">
+        <f aca="false">IF(L113&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V113" s="4"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
@@ -5682,6 +6265,11 @@
       <c r="M114" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="N114" s="0" t="n">
+        <f aca="false">IF(L114&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V114" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5702,12 +6290,12 @@
   <dimension ref="A1:T114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="V:V P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,10 +6380,10 @@
       <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
         <v>113</v>
       </c>
     </row>
@@ -5840,10 +6428,10 @@
       <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="2" t="n">
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <f aca="false">SUM(M2:M114)</f>
         <v>23</v>
       </c>
@@ -5889,10 +6477,10 @@
       <c r="M4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2" t="n">
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <f aca="false">P3/P2</f>
         <v>0.20353982300885</v>
       </c>
@@ -5938,10 +6526,10 @@
       <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="n">
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -5986,24 +6574,24 @@
       <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2" t="n">
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <f aca="false">P5*P4</f>
         <v>2.44247787610619</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2" t="n">
+      <c r="Q6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <f aca="false">(P3/P2)*(1 - (P3/P2))*P5*((P2-P5)/(P2-1))</f>
         <v>1.75427654028171</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="2" t="n">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="3" t="n">
         <f aca="false">SQRT(R6)</f>
         <v>1.32449104952873</v>
       </c>
@@ -6049,19 +6637,19 @@
       <c r="M7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="O7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <f aca="false">COUNTIF(M2:M13, "=1")</f>
         <v>5</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="n">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3" t="n">
         <f aca="false">P6+2*T6</f>
         <v>5.09145997516365</v>
       </c>
@@ -6107,10 +6695,10 @@
       <c r="M8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -6153,17 +6741,17 @@
       <c r="M9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="O9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="n">
         <f aca="false">P7/P6 - 1</f>
         <v>1.04710144927536</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -6249,13 +6837,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10713,12 +11301,12 @@
   <dimension ref="A1:T114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="V:V P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10803,10 +11391,10 @@
       <c r="M2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
         <v>113</v>
       </c>
     </row>
@@ -10851,10 +11439,10 @@
       <c r="M3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="2" t="n">
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <f aca="false">SUM(M2:M114)</f>
         <v>20</v>
       </c>
@@ -10900,10 +11488,10 @@
       <c r="M4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2" t="n">
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <f aca="false">P3/P2</f>
         <v>0.176991150442478</v>
       </c>
@@ -10949,10 +11537,10 @@
       <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="n">
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -10997,24 +11585,24 @@
       <c r="M6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2" t="n">
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <f aca="false">P5*P4</f>
         <v>2.12389380530973</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2" t="n">
+      <c r="Q6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <f aca="false">(P3/P2)*(1 - (P3/P2))*P5*((P2-P5)/(P2-1))</f>
         <v>1.57630645648501</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="2" t="n">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="3" t="n">
         <f aca="false">SQRT(R6)</f>
         <v>1.25551043662927</v>
       </c>
@@ -11060,19 +11648,19 @@
       <c r="M7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="O7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <f aca="false">COUNTIF(M2:M13, "=1")</f>
         <v>5</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="n">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3" t="n">
         <f aca="false">P6+2*T6</f>
         <v>4.63491467856827</v>
       </c>
@@ -11118,10 +11706,10 @@
       <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -11164,17 +11752,17 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="O9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="n">
         <f aca="false">P7/P6 - 1</f>
         <v>1.35416666666667</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -11260,13 +11848,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15724,12 +16312,12 @@
   <dimension ref="A1:T114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="V:V P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15814,10 +16402,10 @@
       <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
         <v>113</v>
       </c>
     </row>
@@ -15862,10 +16450,10 @@
       <c r="M3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="2" t="n">
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <f aca="false">SUM(M2:M114)</f>
         <v>23</v>
       </c>
@@ -15911,10 +16499,10 @@
       <c r="M4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2" t="n">
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <f aca="false">P3/P2</f>
         <v>0.20353982300885</v>
       </c>
@@ -15960,10 +16548,10 @@
       <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="n">
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -16008,24 +16596,24 @@
       <c r="M6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2" t="n">
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <f aca="false">P5*P4</f>
         <v>2.44247787610619</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2" t="n">
+      <c r="Q6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <f aca="false">(P3/P2)*(1 - (P3/P2))*P5*((P2-P5)/(P2-1))</f>
         <v>1.75427654028171</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="2" t="n">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="3" t="n">
         <f aca="false">SQRT(R6)</f>
         <v>1.32449104952873</v>
       </c>
@@ -16071,19 +16659,19 @@
       <c r="M7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="O7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <f aca="false">COUNTIF(M2:M13, "=1")</f>
         <v>6</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="n">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3" t="n">
         <f aca="false">P6+2*T6</f>
         <v>5.09145997516365</v>
       </c>
@@ -16129,10 +16717,10 @@
       <c r="M8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -16175,17 +16763,17 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="O9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="n">
         <f aca="false">P7/P6 - 1</f>
         <v>1.45652173913043</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -16271,13 +16859,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20735,12 +21323,12 @@
   <dimension ref="A1:T114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
+      <selection pane="topLeft" activeCell="P12" activeCellId="1" sqref="V:V P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20825,10 +21413,10 @@
       <c r="M2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="2" t="n">
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
         <v>113</v>
       </c>
     </row>
@@ -20873,10 +21461,10 @@
       <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="2" t="n">
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="n">
         <f aca="false">SUM(M2:M114)</f>
         <v>22</v>
       </c>
@@ -20922,10 +21510,10 @@
       <c r="M4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2" t="n">
+      <c r="O4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="3" t="n">
         <f aca="false">P3/P2</f>
         <v>0.194690265486726</v>
       </c>
@@ -20971,10 +21559,10 @@
       <c r="M5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2" t="n">
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3" t="n">
         <v>12</v>
       </c>
     </row>
@@ -21019,24 +21607,24 @@
       <c r="M6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2" t="n">
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="n">
         <f aca="false">P5*P4</f>
         <v>2.33628318584071</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="2" t="n">
+      <c r="Q6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="3" t="n">
         <f aca="false">(P3/P2)*(1 - (P3/P2))*P5*((P2-P5)/(P2-1))</f>
         <v>1.69664813219516</v>
       </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="2" t="n">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="3" t="n">
         <f aca="false">SQRT(R6)</f>
         <v>1.30255446419532</v>
       </c>
@@ -21082,19 +21670,19 @@
       <c r="M7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="2" t="n">
+      <c r="O7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="n">
         <f aca="false">COUNTIF(M2:M13, "=1")</f>
         <v>6</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="n">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3" t="n">
         <f aca="false">P6+2*T6</f>
         <v>4.94139211423135</v>
       </c>
@@ -21140,10 +21728,10 @@
       <c r="M8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -21186,17 +21774,17 @@
       <c r="M9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="3" t="n">
+      <c r="O9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="n">
         <f aca="false">P7/P6 - 1</f>
         <v>1.56818181818182</v>
       </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -21282,13 +21870,13 @@
         <v>1</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25746,23 +26334,23 @@
   <dimension ref="B2:P12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+      <selection pane="topLeft" activeCell="O27" activeCellId="1" sqref="V:V O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>